<commit_message>
marco segmentos incluidos en area motora primaria
</commit_message>
<xml_diff>
--- a/segmentos.xlsx
+++ b/segmentos.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
   <si>
     <t>Segment</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>ctx-rh-insula</t>
+  </si>
+  <si>
+    <t>VALOR</t>
   </si>
 </sst>
 </file>
@@ -480,12 +483,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -500,9 +509,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A110" sqref="A2:A110"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +812,7 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -814,8 +825,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -828,8 +842,11 @@
       <c r="D2" s="1">
         <v>219574</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -842,8 +859,11 @@
       <c r="D3" s="1">
         <v>3008</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -856,8 +876,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -870,8 +893,11 @@
       <c r="D5" s="1">
         <v>12362</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -884,8 +910,11 @@
       <c r="D6" s="1">
         <v>50302</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -898,8 +927,11 @@
       <c r="D7" s="1">
         <v>8749</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -912,8 +944,11 @@
       <c r="D8" s="1">
         <v>3103</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -926,8 +961,11 @@
       <c r="D9" s="1">
         <v>5127</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -940,8 +978,11 @@
       <c r="D10" s="1">
         <v>1976</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -954,8 +995,11 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -968,8 +1012,11 @@
       <c r="D12" s="1">
         <v>1594</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -982,8 +1029,11 @@
       <c r="D13" s="1">
         <v>19863</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -996,8 +1046,11 @@
       <c r="D14" s="1">
         <v>4264</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1010,8 +1063,11 @@
       <c r="D15" s="1">
         <v>1634</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1024,8 +1080,11 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1038,8 +1097,11 @@
       <c r="D17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1052,8 +1114,11 @@
       <c r="D18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1066,8 +1131,11 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1080,8 +1148,11 @@
       <c r="D20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1094,8 +1165,11 @@
       <c r="D21" s="1">
         <v>217376</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1108,8 +1182,11 @@
       <c r="D22" s="1">
         <v>2879</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1122,8 +1199,11 @@
       <c r="D23" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1136,8 +1216,11 @@
       <c r="D24" s="1">
         <v>12152</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1150,8 +1233,11 @@
       <c r="D25" s="1">
         <v>51916</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1164,8 +1250,11 @@
       <c r="D26" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1178,8 +1267,11 @@
       <c r="D27" s="1">
         <v>3216</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1192,8 +1284,11 @@
       <c r="D28" s="1">
         <v>5291</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1206,8 +1301,11 @@
       <c r="D29" s="1">
         <v>1859</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1220,8 +1318,11 @@
       <c r="D30" s="1">
         <v>4917</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -1234,8 +1335,11 @@
       <c r="D31" s="1">
         <v>1675</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1248,8 +1352,11 @@
       <c r="D32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1262,8 +1369,11 @@
       <c r="D33" s="1">
         <v>4225</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1276,8 +1386,11 @@
       <c r="D34" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -1290,8 +1403,11 @@
       <c r="D35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1304,8 +1420,11 @@
       <c r="D36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1318,8 +1437,11 @@
       <c r="D37" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1332,8 +1454,11 @@
       <c r="D38" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -1346,8 +1471,11 @@
       <c r="D39" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1360,8 +1488,11 @@
       <c r="D40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -1374,8 +1505,11 @@
       <c r="D41" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -1388,8 +1522,11 @@
       <c r="D42" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -1402,8 +1539,11 @@
       <c r="D43" s="1">
         <v>2506</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -1416,8 +1556,11 @@
       <c r="D44" s="1">
         <v>2114</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -1430,8 +1573,11 @@
       <c r="D45" s="1">
         <v>6202</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -1444,8 +1590,11 @@
       <c r="D46" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -1458,8 +1607,11 @@
       <c r="D47" s="1">
         <v>2075</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1472,8 +1624,11 @@
       <c r="D48" s="1">
         <v>9663</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -1486,8 +1641,11 @@
       <c r="D49" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -1500,8 +1658,11 @@
       <c r="D50" s="1">
         <v>11184</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -1514,8 +1675,11 @@
       <c r="D51" s="1">
         <v>2463</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>75</v>
       </c>
@@ -1528,8 +1692,11 @@
       <c r="D52" s="1">
         <v>12055</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -1542,8 +1709,11 @@
       <c r="D53" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -1556,8 +1726,11 @@
       <c r="D54" s="1">
         <v>6106</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -1570,8 +1743,11 @@
       <c r="D55" s="1">
         <v>5359</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>80</v>
       </c>
@@ -1584,8 +1760,11 @@
       <c r="D56" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -1598,22 +1777,28 @@
       <c r="D57" s="1">
         <v>2516</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="E57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="2">
         <v>3783</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>3783</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="3">
         <v>3783</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -1626,8 +1811,11 @@
       <c r="D59" s="1">
         <v>3891</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>85</v>
       </c>
@@ -1640,8 +1828,11 @@
       <c r="D60" s="1">
         <v>2215</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -1654,8 +1845,11 @@
       <c r="D61" s="1">
         <v>3519</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -1668,8 +1862,11 @@
       <c r="D62" s="1">
         <v>2639</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -1682,8 +1879,11 @@
       <c r="D63" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -1696,22 +1896,28 @@
       <c r="D64" s="1">
         <v>3416</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="E64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="2">
         <v>13388</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="2">
         <v>13388</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="3">
         <v>13388</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>92</v>
       </c>
@@ -1724,8 +1930,11 @@
       <c r="D66" s="1">
         <v>10444</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>93</v>
       </c>
@@ -1738,8 +1947,11 @@
       <c r="D67" s="1">
         <v>2239</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>94</v>
       </c>
@@ -1752,8 +1964,11 @@
       <c r="D68" s="1">
         <v>13476</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>95</v>
       </c>
@@ -1766,8 +1981,11 @@
       <c r="D69" s="1">
         <v>23878</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>96</v>
       </c>
@@ -1780,8 +1998,11 @@
       <c r="D70" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -1794,8 +2015,11 @@
       <c r="D71" s="1">
         <v>14112</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>99</v>
       </c>
@@ -1808,8 +2032,11 @@
       <c r="D72" s="1">
         <v>10531</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>100</v>
       </c>
@@ -1822,8 +2049,11 @@
       <c r="D73" s="1">
         <v>1058</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>101</v>
       </c>
@@ -1836,8 +2066,11 @@
       <c r="D74" s="1">
         <v>3208</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>102</v>
       </c>
@@ -1850,8 +2083,11 @@
       <c r="D75" s="1">
         <v>1173</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>103</v>
       </c>
@@ -1864,8 +2100,11 @@
       <c r="D76" s="1">
         <v>6626</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
@@ -1878,8 +2117,11 @@
       <c r="D77" s="1">
         <v>2354</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>105</v>
       </c>
@@ -1892,8 +2134,11 @@
       <c r="D78" s="1">
         <v>2525</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>106</v>
       </c>
@@ -1906,8 +2151,11 @@
       <c r="D79" s="1">
         <v>5449</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>107</v>
       </c>
@@ -1920,8 +2168,11 @@
       <c r="D80" s="1">
         <v>3554</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>108</v>
       </c>
@@ -1934,8 +2185,11 @@
       <c r="D81" s="1">
         <v>2209</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>109</v>
       </c>
@@ -1948,8 +2202,11 @@
       <c r="D82" s="1">
         <v>9954</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>110</v>
       </c>
@@ -1962,8 +2219,11 @@
       <c r="D83" s="1">
         <v>18784</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>111</v>
       </c>
@@ -1976,8 +2236,11 @@
       <c r="D84" s="1">
         <v>10605</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>112</v>
       </c>
@@ -1990,8 +2253,11 @@
       <c r="D85" s="1">
         <v>3311</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>113</v>
       </c>
@@ -2004,8 +2270,11 @@
       <c r="D86" s="1">
         <v>11859</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>114</v>
       </c>
@@ -2018,8 +2287,11 @@
       <c r="D87" s="1">
         <v>7157</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>115</v>
       </c>
@@ -2032,8 +2304,11 @@
       <c r="D88" s="1">
         <v>6577</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>116</v>
       </c>
@@ -2046,8 +2321,11 @@
       <c r="D89" s="1">
         <v>5097</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>117</v>
       </c>
@@ -2060,8 +2338,11 @@
       <c r="D90" s="1">
         <v>13402</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>118</v>
       </c>
@@ -2074,22 +2355,28 @@
       <c r="D91" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="E91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="2">
         <v>3730</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="2">
         <v>3730</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>122</v>
       </c>
@@ -2102,8 +2389,11 @@
       <c r="D93" s="1">
         <v>3736</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>123</v>
       </c>
@@ -2116,8 +2406,11 @@
       <c r="D94" s="1">
         <v>3128</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>124</v>
       </c>
@@ -2130,8 +2423,11 @@
       <c r="D95" s="1">
         <v>4457</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>125</v>
       </c>
@@ -2144,8 +2440,11 @@
       <c r="D96" s="1">
         <v>2781</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>126</v>
       </c>
@@ -2158,8 +2457,11 @@
       <c r="D97" s="1">
         <v>8358</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>127</v>
       </c>
@@ -2172,22 +2474,28 @@
       <c r="D98" s="1">
         <v>3725</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="E98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="2">
         <v>12758</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="2">
         <v>12758</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="3">
         <v>12758</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>129</v>
       </c>
@@ -2200,8 +2508,11 @@
       <c r="D100" s="1">
         <v>11234</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>130</v>
       </c>
@@ -2214,8 +2525,11 @@
       <c r="D101" s="1">
         <v>2208</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>131</v>
       </c>
@@ -2228,8 +2542,11 @@
       <c r="D102" s="1">
         <v>15394</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>132</v>
       </c>
@@ -2242,8 +2559,11 @@
       <c r="D103" s="1">
         <v>21601</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>133</v>
       </c>
@@ -2256,8 +2576,11 @@
       <c r="D104" s="1">
         <v>13582</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>134</v>
       </c>
@@ -2270,8 +2593,11 @@
       <c r="D105" s="1">
         <v>12298</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>135</v>
       </c>
@@ -2284,8 +2610,11 @@
       <c r="D106" s="1">
         <v>9956</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>136</v>
       </c>
@@ -2298,8 +2627,11 @@
       <c r="D107" s="1">
         <v>1275</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>137</v>
       </c>
@@ -2312,8 +2644,11 @@
       <c r="D108" s="1">
         <v>2867</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>138</v>
       </c>
@@ -2326,8 +2661,11 @@
       <c r="D109" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>140</v>
       </c>
@@ -2339,6 +2677,9 @@
       </c>
       <c r="D110" s="1">
         <v>7171</v>
+      </c>
+      <c r="E110">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>